<commit_message>
Final project rough draft
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/md990a/UTD_2019_Spring/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6668114F-BE18-3B4A-AFC2-18E2355B1DA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36800" yWindow="-760" windowWidth="24480" windowHeight="15120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24480" windowHeight="15120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="Grade Cutoffs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -139,9 +145,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -242,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -251,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -285,6 +291,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -609,14 +623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -626,7 +640,7 @@
     <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -646,7 +660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -664,7 +678,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
         <v>43121</v>
@@ -676,7 +690,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -696,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -716,7 +730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -736,7 +750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -754,7 +768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -770,7 +784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -790,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -808,7 +822,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5">
         <v>43177</v>
@@ -820,7 +834,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -838,7 +852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -852,7 +866,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -870,7 +884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -886,7 +900,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -902,7 +916,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -916,7 +930,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -943,16 +957,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -960,7 +974,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -968,7 +982,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -976,12 +990,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>

</xml_diff>